<commit_message>
Fix - indexación nuevos nombres
</commit_message>
<xml_diff>
--- a/Procesamiento/Excel/Papers con informacion.xlsx
+++ b/Procesamiento/Excel/Papers con informacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\Github\BRI - Buscador medico\Procesamiento\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ED3A14-9B61-4A61-86CD-E4481B2EE1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913C3C13-1630-4678-9BA3-41D34F0FC049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,9 +171,6 @@
     <t>https://www.cdc.gov/std/chlamydia/default.htm</t>
   </si>
   <si>
-    <t>Cistitis_ diagnóstico, tratamiento y prevención de recidivas</t>
-  </si>
-  <si>
     <t>FACULTAD DE FARMACIA
 UNIVERSIDAD COMPLUTENSE DE MADRID</t>
   </si>
@@ -227,9 +224,6 @@
   </si>
   <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6492228/</t>
-  </si>
-  <si>
-    <t>Concepto de sospecha de glaucoma de ángulo abierto_ definición, diagnóstico y tratamiento</t>
   </si>
   <si>
     <t>Revista Mexicana de Oftalmología</t>
@@ -550,9 +544,6 @@
     <t>https://www-sciencedirect-com.ezproxy.usach.cl/science/article/pii/S0165032708003492?via%3Dihub</t>
   </si>
   <si>
-    <t>Ebola_ a review on the state of the art on prevention and treatment</t>
-  </si>
-  <si>
     <t>Asian Pacific Journal of Tropical Biomedicine</t>
   </si>
   <si>
@@ -586,9 +577,6 @@
     <t>https://onlinelibrary-wiley-com.ezproxy.usach.cl/doi/10.1111/joor.12380</t>
   </si>
   <si>
-    <t>Encefalitis_ ¿cuáles y cómo tratar_</t>
-  </si>
-  <si>
     <t>Revista Chilena de Infectología</t>
   </si>
   <si>
@@ -604,9 +592,6 @@
     <t>https://www.scielo.cl/scielo.php?pid=S0716-10182003020100004&amp;script=sci_arttext&amp;tlng=pt</t>
   </si>
   <si>
-    <t>Endometriosis_ diagnóstico y alternativas terapéuticas</t>
-  </si>
-  <si>
     <t>Pereira, J., Pereira, Y. &amp; Quirós L.</t>
   </si>
   <si>
@@ -617,9 +602,6 @@
   </si>
   <si>
     <t>https://revistamedicasinergia.com/index.php/rms/article/view/361/721</t>
-  </si>
-  <si>
-    <t>Enfermedad Gota_ Revisión Bibliográfica</t>
   </si>
   <si>
     <t>Revista Ciencia &amp; Salud: Integrando Conocimientos</t>
@@ -731,9 +713,6 @@
     <t>https://www-sciencedirect-com.ezproxy.usach.cl/science/article/pii/S2352250X20302153?via%3Dihub</t>
   </si>
   <si>
-    <t>Gonorrhea_ Treatment update for an incresaingly resistan organism</t>
-  </si>
-  <si>
     <t>PubMed</t>
   </si>
   <si>
@@ -884,9 +863,6 @@
     <t>https://ccforum.biomedcentral.com/articles/10.1186/s13054-019-2491-9</t>
   </si>
   <si>
-    <t>Influenza_ vaccination and treatment</t>
-  </si>
-  <si>
     <t>European Respiratory Journal</t>
   </si>
   <si>
@@ -902,18 +878,12 @@
     <t>https://erj.ersjournals.com/content/erj/17/6/1282.full.pdf</t>
   </si>
   <si>
-    <t>Información básica sobre la hemofilia _ Hemofilia _ NCBDDD _ CDC</t>
-  </si>
-  <si>
     <t>Centers for Disease Control and Prevention</t>
   </si>
   <si>
     <t>https://www.cdc.gov/ncbddd/hemophilia/index.html</t>
   </si>
   <si>
-    <t>Leprosy – an overview of clinical features, diagnosis, and treatment</t>
-  </si>
-  <si>
     <t>Journal der Deutschen Dermatologischen Gesellschaf</t>
   </si>
   <si>
@@ -926,9 +896,6 @@
     <t>https://onlinelibrary.wiley.com/doi/full/10.1111/ddg.13301?casa_token=vXEO4y71SnoAAAAA%3AGpL5Y6AZiAQpnwfSUNGDi9rl20F0iBzruuc36wqJ4A2AXW9PHdh79QvRVdJPunvSoDCv6xAaUl4bDVQ</t>
   </si>
   <si>
-    <t>Lung cancer_ biology and treatment options</t>
-  </si>
-  <si>
     <t>Biochim Biophys Acta.</t>
   </si>
   <si>
@@ -942,9 +909,6 @@
   </si>
   <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4663145/</t>
-  </si>
-  <si>
-    <t>Lupus_ An Overview of the Disease And Management Options</t>
   </si>
   <si>
     <t>Pharmacy and Therapeutics</t>
@@ -1164,9 +1128,6 @@
     <t>https://jeatdisord.biomedcentral.com/articles/10.1186/s40337-023-00758-3</t>
   </si>
   <si>
-    <t>Prevention _ E. coli _ CDC</t>
-  </si>
-  <si>
     <t>U.S Department of Health &amp; Human Services</t>
   </si>
   <si>
@@ -1238,9 +1199,6 @@
     <t>https://www.hindawi.com/journals/tswj/2006/936460/</t>
   </si>
   <si>
-    <t>Rheumatoid Arthritis_ A Brief Overview of the Treatment</t>
-  </si>
-  <si>
     <t>Medical Principles and Practical</t>
   </si>
   <si>
@@ -1274,9 +1232,6 @@
     <t>https://editorial.ucsg.edu.ec/ojs-medicina/index.php/ucsg-medicina/article/view/301/262</t>
   </si>
   <si>
-    <t>Salmonella_infection_-_prevention_and_treatment_by-1</t>
-  </si>
-  <si>
     <t>Microbiology</t>
   </si>
   <si>
@@ -1511,9 +1466,6 @@
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC7223059/</t>
   </si>
   <si>
-    <t>Treatment of Hemophilia _ CDC</t>
-  </si>
-  <si>
     <t>U.S. Department of Health &amp; Human Services</t>
   </si>
   <si>
@@ -1577,9 +1529,6 @@
     <t>https://www-tandfonline-com.ezproxy.usach.cl/doi/full/10.1111/j.1444-0938.2007.00211.x</t>
   </si>
   <si>
-    <t>vsr</t>
-  </si>
-  <si>
     <t>Dominio de las Ciencias</t>
   </si>
   <si>
@@ -1595,10 +1544,61 @@
     <t>https://www.dominiodelasciencias.com/ojs/index.php/es/article/view/1857</t>
   </si>
   <si>
-    <t>What is Hemophilia _ CDC</t>
-  </si>
-  <si>
     <t>Hemophilia is usually an inherited bleeding disorder in which the blood does not clot properly. This can lead to spontaneous bleeding as well as bleeding following injuries or surgery. Blood contains many  proteins called clotting factors that can help to stop bleeding. People with hemophilia have low levels of either factor VIII (8) or factor IX (9). The severity of hemophilia that a person has is determined by the amount of factor in the blood. The lower the amount of the factor, the more likely it is that bleeding will occur which can lead to serious health problems. In rare cases, a person can develop hemophilia later in life.  The  majority of cases involve middle-aged or elderly people, or young women  who have recently given birth or are in the later stages of pregnancy. This condition often resolves with appropriate treatment.</t>
+  </si>
+  <si>
+    <t>Cistitis diagnóstico, tratamiento y prevención de recidivas</t>
+  </si>
+  <si>
+    <t>Concepto de sospecha de glaucoma de ángulo abierto definición, diagnóstico y tratamiento</t>
+  </si>
+  <si>
+    <t>Ebola a review on the state of the art on prevention and treatment</t>
+  </si>
+  <si>
+    <t>Encefalitis cuáles y cómo tratar</t>
+  </si>
+  <si>
+    <t>Endometriosis diagnóstico y alternativas terapéuticas</t>
+  </si>
+  <si>
+    <t>Enfermedad Gota Revisión Bibliográfica</t>
+  </si>
+  <si>
+    <t>Gonorrhea Treatment update for an incresaingly resistan organism</t>
+  </si>
+  <si>
+    <t>Influenza vaccination and treatment</t>
+  </si>
+  <si>
+    <t>Información básica sobre la hemofilia Hemofilia NCBDDD CDC</t>
+  </si>
+  <si>
+    <t>Leprosy an overview of clinical features, diagnosis, and treatment</t>
+  </si>
+  <si>
+    <t>Lung cancer biology and treatment options</t>
+  </si>
+  <si>
+    <t>Lupus An Overview of the Disease And Management Options</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Rheumatoid Arthritis A Brief Overview of the Treatment</t>
+  </si>
+  <si>
+    <t>Salmonella infection prevention and treatment</t>
+  </si>
+  <si>
+    <t>Treatment of Hemophilia</t>
+  </si>
+  <si>
+    <t>Virus respiratorio sincitial</t>
+  </si>
+  <si>
+    <t>What is Hemophilia</t>
   </si>
 </sst>
 </file>
@@ -1939,8 +1939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2154,251 +2154,251 @@
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="D9" s="13">
         <v>2015</v>
       </c>
       <c r="E9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="G9" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="H9" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="D10" s="13">
         <v>2009</v>
       </c>
       <c r="E10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="D11" s="13">
         <v>2019</v>
       </c>
       <c r="E11" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>64</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="D12" s="13">
         <v>2014</v>
       </c>
       <c r="E12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="D13" s="13">
         <v>2009</v>
       </c>
       <c r="E13" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="D14" s="13">
         <v>2016</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="D15" s="13">
         <v>2015</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="D16" s="13">
         <v>2020</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>98</v>
       </c>
       <c r="D17" s="13">
         <v>2016</v>
       </c>
       <c r="E17" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="13">
         <v>2021</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
@@ -2410,579 +2410,579 @@
     </row>
     <row r="19" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>107</v>
       </c>
       <c r="D19" s="13">
         <v>2010</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="D20" s="13">
         <v>2012</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D21" s="13">
         <v>2010</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>120</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>122</v>
       </c>
       <c r="D22" s="13">
         <v>2017</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="D23" s="13">
         <v>2008</v>
       </c>
       <c r="E23" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>134</v>
       </c>
       <c r="D24" s="13">
         <v>2002</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="D25" s="13">
         <v>2007</v>
       </c>
       <c r="E25" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>143</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>145</v>
       </c>
       <c r="D26" s="13">
         <v>2020</v>
       </c>
       <c r="E26" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="D27" s="13">
         <v>2020</v>
       </c>
       <c r="E27" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>157</v>
       </c>
       <c r="D28" s="13">
         <v>2013</v>
       </c>
       <c r="E28" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D29" s="13">
         <v>2017</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>166</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>168</v>
       </c>
       <c r="D30" s="13">
         <v>2009</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>172</v>
+        <v>504</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D31" s="13">
         <v>2014</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D32" s="13">
         <v>2016</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
-        <v>184</v>
+        <v>505</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D33" s="13">
         <v>2003</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
-        <v>190</v>
+        <v>506</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D34" s="13">
         <v>2020</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>195</v>
+        <v>507</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D35" s="13">
         <v>2020</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D36" s="13">
         <v>2013</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D37" s="13">
         <v>2012</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D38" s="13">
         <v>2013</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D39" s="13">
         <v>2010</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D40" s="13">
         <v>2021</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>231</v>
+        <v>508</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D41" s="13">
         <v>2015</v>
@@ -2993,44 +2993,44 @@
         <v>13</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D42" s="13">
         <v>2018</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D43" s="13">
         <v>2010</v>
@@ -3041,16 +3041,16 @@
         <v>13</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="12" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D44" s="13">
         <v>2007</v>
@@ -3058,21 +3058,21 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D45" s="13">
         <v>2018</v>
@@ -3080,21 +3080,21 @@
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D46" s="13">
         <v>2007</v>
@@ -3102,121 +3102,121 @@
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D47" s="13">
         <v>2005</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D48" s="13">
         <v>2021</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D49" s="13">
         <v>2008</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D50" s="13">
         <v>2019</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D51" s="13">
         <v>2018</v>
@@ -3227,41 +3227,41 @@
         <v>13</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
-        <v>282</v>
+        <v>509</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D52" s="13">
         <v>2001</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="G52" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
-        <v>288</v>
+        <v>510</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="13">
@@ -3270,95 +3270,95 @@
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
       <c r="G53" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
-        <v>291</v>
+        <v>511</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D54" s="13">
         <v>2017</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
-        <v>296</v>
+        <v>512</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="D55" s="13">
         <v>2015</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="G55" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="11" t="s">
-        <v>302</v>
+        <v>513</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="D56" s="13">
         <v>2012</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="F56" s="12"/>
       <c r="G56" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="D57" s="13">
         <v>2006</v>
@@ -3366,97 +3366,97 @@
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="11" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="D58" s="13">
         <v>2015</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="G58" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="D59" s="13">
         <v>2021</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="G59" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="D60" s="13">
         <v>2022</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="G60" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="12" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="D61" s="13">
         <v>2015</v>
@@ -3464,145 +3464,145 @@
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="D62" s="13">
         <v>2016</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="D63" s="13">
         <v>2009</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="G63" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="D64" s="13">
         <v>2000</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="F64" s="12"/>
       <c r="G64" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="D65" s="13">
         <v>2009</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="F65" s="12"/>
       <c r="G65" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="D66" s="13">
         <v>1996</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="G66" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="11" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="B67" s="12"/>
       <c r="C67" s="12" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="D67" s="13">
         <v>1945</v>
@@ -3610,39 +3610,39 @@
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
       <c r="G67" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="11" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="D68" s="13">
         <v>2020</v>
       </c>
       <c r="E68" s="12"/>
       <c r="F68" s="12" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="G68" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
@@ -3651,114 +3651,114 @@
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
       <c r="H69" s="3" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="D70" s="13">
         <v>2023</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="G70" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
-        <v>375</v>
+        <v>514</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="D71" s="13">
         <v>2017</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="F71" s="12"/>
       <c r="G71" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="D72" s="13">
         <v>2014</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="G72" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="D73" s="13">
         <v>2012</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="G73" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="75" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
@@ -3781,314 +3781,314 @@
       <c r="F75" s="12"/>
       <c r="G75" s="12"/>
       <c r="H75" s="3" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="D76" s="13">
         <v>2006</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="F76" s="12"/>
       <c r="G76" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="11" t="s">
-        <v>399</v>
+        <v>515</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="D77" s="13">
         <v>2018</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="G77" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="11" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="D78" s="13">
         <v>2006</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="11" t="s">
-        <v>411</v>
+        <v>516</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="D79" s="13">
         <v>2018</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="G79" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="11" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D80" s="13">
         <v>2019</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="G80" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="D81" s="13">
         <v>1994</v>
       </c>
       <c r="E81" s="12"/>
       <c r="F81" s="12" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="G81" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="D82" s="13">
         <v>2018</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="G82" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="11" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="D83" s="13">
         <v>2008</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="G83" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="11" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="D84" s="13">
         <v>2005</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="11" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="D85" s="13">
         <v>1992</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="F85" s="12"/>
       <c r="G85" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="11" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="D86" s="13">
         <v>2005</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="F86" s="12"/>
       <c r="G86" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="11" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="D87" s="17">
         <v>2017</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="F87" s="12"/>
       <c r="G87" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="11" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
@@ -4097,90 +4097,90 @@
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
       <c r="H88" s="3" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="D89" s="13">
         <v>2016</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="F89" s="12"/>
       <c r="G89" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="11" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="D90" s="13">
         <v>2003</v>
       </c>
       <c r="E90" s="12" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="F90" s="12"/>
       <c r="G90" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="11" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="D91" s="13">
         <v>2013</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="F91" s="12"/>
       <c r="G91" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="11" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D92" s="13">
         <v>2022</v>
@@ -4191,160 +4191,160 @@
         <v>13</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="11" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="B93" s="12"/>
       <c r="C93" s="12" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="D93" s="13">
         <v>2022</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="F93" s="12"/>
       <c r="G93" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="11" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="D94" s="13">
         <v>2020</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="11" t="s">
-        <v>490</v>
+        <v>517</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="D95" s="13">
         <v>2022</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
       <c r="F95" s="12"/>
       <c r="G95" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="11" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="D96" s="13">
         <v>2002</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="F96" s="12" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="G96" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="11" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="D97" s="13">
         <v>1999</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
       <c r="F97" s="12"/>
       <c r="G97" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="11" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="D98" s="13">
         <v>2022</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="G98" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="11" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
@@ -4353,57 +4353,57 @@
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
       <c r="H99" s="3" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="11" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
       <c r="D100" s="13">
         <v>2021</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>515</v>
+        <v>498</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
       <c r="G100" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>517</v>
+        <v>500</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="11" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="D101" s="13">
         <v>2022</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="F101" s="12"/>
       <c r="G101" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>